<commit_message>
Tests for expanding range.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/RangeTests.xlsx
+++ b/test/Table_Tests/data/RangeTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57351D50-C5F2-47B6-BDDE-A3CEC84204D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9122AFB-F141-426B-8259-0A7E47E157B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15450" yWindow="-16530" windowWidth="29040" windowHeight="15720" xr2:uid="{D5A689EC-9CFD-4852-A8D3-28F242ADAAC0}"/>
+    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D5A689EC-9CFD-4852-A8D3-28F242ADAAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Extend</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>BB</t>
   </si>
 </sst>
 </file>
@@ -444,17 +450,17 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Additional tests for warnings.
</commit_message>
<xml_diff>
--- a/test/Table_Tests/data/RangeTests.xlsx
+++ b/test/Table_Tests/data/RangeTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enso\ide\test\Table_Tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9122AFB-F141-426B-8259-0A7E47E157B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A19579-41A1-4ECC-B581-6CFD439041E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13350" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D5A689EC-9CFD-4852-A8D3-28F242ADAAC0}"/>
+    <workbookView xWindow="15450" yWindow="-16530" windowWidth="29040" windowHeight="15720" xr2:uid="{D5A689EC-9CFD-4852-A8D3-28F242ADAAC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>BB</t>
+  </si>
+  <si>
+    <t>DD</t>
   </si>
 </sst>
 </file>
@@ -447,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEEB6EE-578B-4B65-BC80-21B1C08A02E2}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -489,8 +492,14 @@
       <c r="P1" t="s">
         <v>11</v>
       </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -515,8 +524,14 @@
       <c r="P2">
         <v>2</v>
       </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -535,8 +550,14 @@
       <c r="P3">
         <v>2</v>
       </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -559,7 +580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -579,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -587,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>